<commit_message>
Pushing code for OrangeHRM
</commit_message>
<xml_diff>
--- a/TestDataSheet/OrangeHRM.xlsx
+++ b/TestDataSheet/OrangeHRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IntellijProjectWorkSpace\Project6\TestDataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02B24EE-9356-4F93-B13E-E88B36EEF410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07408DE0-786E-4349-B451-FA766EBA3424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4632" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeHRM" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>